<commit_message>
Definicion de REST WS
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/MapeoWS.xlsx
+++ b/DOCUMENTACION/MapeoWS.xlsx
@@ -4,20 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="555" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>CAFETERIAS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
   <si>
     <t xml:space="preserve">RUTA </t>
   </si>
@@ -25,17 +22,134 @@
     <t xml:space="preserve">DESCRIPCIÓN </t>
   </si>
   <si>
-    <t>/spring/rest/cafeterias/{lineaId}</t>
-  </si>
-  <si>
     <t>Devuelve todas las cafeterias pertenecientes a una linea</t>
+  </si>
+  <si>
+    <t>/spring/rest</t>
+  </si>
+  <si>
+    <t>/{lineaId}</t>
+  </si>
+  <si>
+    <t>/cafeterias</t>
+  </si>
+  <si>
+    <t>/plantillas</t>
+  </si>
+  <si>
+    <t>/plazas</t>
+  </si>
+  <si>
+    <t>/empleados</t>
+  </si>
+  <si>
+    <t>/ventas</t>
+  </si>
+  <si>
+    <t>Devuelve la cafeteria con el nombre indicado</t>
+  </si>
+  <si>
+    <t>Crea una nueva cafeteria para la linea</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Elimina la cafeteria especificada del sistema</t>
+  </si>
+  <si>
+    <t>/{cafeteriaId}</t>
+  </si>
+  <si>
+    <t>/delete</t>
+  </si>
+  <si>
+    <t>Método</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Modifica la cafeteria indicada</t>
+  </si>
+  <si>
+    <t>/create</t>
+  </si>
+  <si>
+    <t>/update</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>Id de la cafeteria</t>
+  </si>
+  <si>
+    <t>Id de la linea</t>
+  </si>
+  <si>
+    <t>JSON de la cafeteria con todos los datos</t>
+  </si>
+  <si>
+    <t>JSON Collection con todas las cafeterias</t>
+  </si>
+  <si>
+    <t>Objeto a elminar</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Objeto actualizado</t>
+  </si>
+  <si>
+    <t>Objeto a crear</t>
+  </si>
+  <si>
+    <t>/{lineaId}/{cafeteriaId}</t>
+  </si>
+  <si>
+    <t>/{cafeteriaId}/{plantillaId}</t>
+  </si>
+  <si>
+    <t>/{plantillaId}/{plazaId}</t>
+  </si>
+  <si>
+    <t>/{plantillaId}</t>
+  </si>
+  <si>
+    <t>/{plazaId}</t>
+  </si>
+  <si>
+    <t>/{empleadoId}</t>
+  </si>
+  <si>
+    <t>/{cafeteriaId}/{fechaInicio}/{fechaFin}</t>
+  </si>
+  <si>
+    <t>/reportes</t>
+  </si>
+  <si>
+    <t>/{cafeteriaId}/{empleadoId}</t>
+  </si>
+  <si>
+    <t>/{cafeteriaId}/{reporteId}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,13 +157,134 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,15 +299,108 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -379,45 +707,470 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C4"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="33.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="23"/>
+      <c r="C16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
+      <c r="C18" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
+      <c r="C19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
+      <c r="C20" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="24"/>
+      <c r="C21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="C23" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="25"/>
+      <c r="C24" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="25"/>
+      <c r="C25" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="25"/>
+      <c r="C26" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="26"/>
+      <c r="C28" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="26"/>
+      <c r="C29" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="26"/>
+      <c r="C30" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="26"/>
+      <c r="C31" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+  <mergeCells count="8">
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="B12:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizando proyecto Spring y mapeo de WS
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/MapeoWS.xlsx
+++ b/DOCUMENTACION/MapeoWS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="86">
   <si>
     <t xml:space="preserve">RUTA </t>
   </si>
@@ -25,9 +25,6 @@
     <t>Devuelve todas las cafeterias pertenecientes a una linea</t>
   </si>
   <si>
-    <t>/spring/rest</t>
-  </si>
-  <si>
     <t>/{lineaId}</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>JSON de la cafeteria con todos los datos</t>
   </si>
   <si>
-    <t>JSON Collection con todas las cafeterias</t>
-  </si>
-  <si>
     <t>Objeto a elminar</t>
   </si>
   <si>
@@ -143,13 +137,148 @@
   </si>
   <si>
     <t>/{cafeteriaId}/{reporteId}</t>
+  </si>
+  <si>
+    <t>https://coffesale.herokuapp.com/rest</t>
+  </si>
+  <si>
+    <t>Crea una nueva plantilla para la cafeteria recibida</t>
+  </si>
+  <si>
+    <t>Devuelve una plantilla con el id indicado</t>
+  </si>
+  <si>
+    <t>Id de cafeteria y Id de plantilla</t>
+  </si>
+  <si>
+    <t>Devuelve conjunto de plantillas en la cafeteria indicada</t>
+  </si>
+  <si>
+    <t>Actualiza la información de una plantilla</t>
+  </si>
+  <si>
+    <t>Objeto a eliminar</t>
+  </si>
+  <si>
+    <t>Elimina una plantilla indicada</t>
+  </si>
+  <si>
+    <t>Crea una nueva plaza</t>
+  </si>
+  <si>
+    <t>Devuelve una plaza con id de plaza indicado</t>
+  </si>
+  <si>
+    <t>Id de la plaza y Id de la plantilla</t>
+  </si>
+  <si>
+    <t>Devuelve conjunto de plazas para la plantilla indicada</t>
+  </si>
+  <si>
+    <t>JSON de la plantilla con todos los datos</t>
+  </si>
+  <si>
+    <t>JSON de la plaza con todos los datos</t>
+  </si>
+  <si>
+    <t>JSON Collection con todas las plazas de la plantilla</t>
+  </si>
+  <si>
+    <t>JSON Collection con todas las plantillas de la cafeteria</t>
+  </si>
+  <si>
+    <t>JSON Collection con todas las cafeterias de la linea</t>
+  </si>
+  <si>
+    <t>Actualiza la información de una plaza</t>
+  </si>
+  <si>
+    <t>Id de la plantilla</t>
+  </si>
+  <si>
+    <t>Elimina una plaza indicada</t>
+  </si>
+  <si>
+    <t>Crea un nuevo empleado</t>
+  </si>
+  <si>
+    <t>Devuelve al empleado trabajando en laplaza indicada</t>
+  </si>
+  <si>
+    <t>Devuelve los datos del empleado indicado</t>
+  </si>
+  <si>
+    <t>Id de la plaza donde labora el empleado</t>
+  </si>
+  <si>
+    <t>Id del empleado</t>
+  </si>
+  <si>
+    <t>JSON del empleado con sus datos completos</t>
+  </si>
+  <si>
+    <t>Actualiza la información de un empleado</t>
+  </si>
+  <si>
+    <t>Elimina un empleado</t>
+  </si>
+  <si>
+    <t>Genera un nuevo registro de venta</t>
+  </si>
+  <si>
+    <t>Devuelve las ventas de una cafeteria en un intervalo cerrado</t>
+  </si>
+  <si>
+    <t>Id de la cafeteria que se leerá, la fecha desde la que se leerá y la fecha de termino</t>
+  </si>
+  <si>
+    <t>JSON Collection con todas las ventas que incidan en el rango de fechas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devuelve todas las ventas registradas en una cafeteria ese mismo dia </t>
+  </si>
+  <si>
+    <t>JSON Collection de las ventas registradas a lo largo del día</t>
+  </si>
+  <si>
+    <t>Actualiza la información de una venta</t>
+  </si>
+  <si>
+    <t>Elimina una venta</t>
+  </si>
+  <si>
+    <t>Crea un nuevo reporte de fallo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devuelve el reporte vigente generado por un empleado específico </t>
+  </si>
+  <si>
+    <t>Id de la cafeteria y Id del empleado que genero el reporte</t>
+  </si>
+  <si>
+    <t>JSON con los datos del reporte</t>
+  </si>
+  <si>
+    <t>Devuelve conjunto de reportes que coincidan con el tipo de reporte solicitado</t>
+  </si>
+  <si>
+    <t>Id de la cafeteria y Id del reporte (sistema o fallo)</t>
+  </si>
+  <si>
+    <t>JSON Collection con todos los reportes que coincidan</t>
+  </si>
+  <si>
+    <t>Actualiza la información de un reporte</t>
+  </si>
+  <si>
+    <t>Elimina un reporte del sistema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +293,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="21">
     <fill>
@@ -296,8 +433,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -349,36 +487,12 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -403,8 +517,33 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -710,456 +849,623 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="1" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="F2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="34"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="D9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G10" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="3" t="s">
+      <c r="G12" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="D22" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="F26" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
+      <c r="B27" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="5" t="s">
+      <c r="G27" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="34"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="34"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21" t="s">
+      <c r="D30" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="7" t="s">
+      <c r="F30" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="34"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21" t="s">
+      <c r="D31" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="24"/>
-      <c r="C19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="24"/>
-      <c r="C21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
-      <c r="C23" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="25"/>
-      <c r="C24" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="25"/>
-      <c r="C25" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="25"/>
-      <c r="C26" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="26"/>
-      <c r="C28" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="26"/>
-      <c r="C29" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="26"/>
-      <c r="C30" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="26"/>
-      <c r="C31" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="F31" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1169,10 +1475,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A2:A15"/>
     <mergeCell ref="B12:B16"/>
+    <mergeCell ref="A2:A31"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en codigo Spring y mapeo WS
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/MapeoWS.xlsx
+++ b/DOCUMENTACION/MapeoWS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="2805" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="88">
   <si>
     <t xml:space="preserve">RUTA </t>
   </si>
@@ -109,9 +109,6 @@
     <t>Objeto a crear</t>
   </si>
   <si>
-    <t>/{lineaId}/{cafeteriaId}</t>
-  </si>
-  <si>
     <t>/{cafeteriaId}/{plantillaId}</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>/{plantillaId}</t>
   </si>
   <si>
-    <t>/{plazaId}</t>
-  </si>
-  <si>
     <t>/{empleadoId}</t>
   </si>
   <si>
@@ -272,6 +266,18 @@
   </si>
   <si>
     <t>Elimina un reporte del sistema</t>
+  </si>
+  <si>
+    <t>/lineas</t>
+  </si>
+  <si>
+    <t>/{lineaId}/{cafeteriaNombre}</t>
+  </si>
+  <si>
+    <t>Id de la linea y nombre de la cafetería</t>
+  </si>
+  <si>
+    <t>/{cafeteriaId}/{plazaId}</t>
   </si>
 </sst>
 </file>
@@ -437,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -517,6 +523,12 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,9 +539,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -846,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,11 +874,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
@@ -884,14 +893,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>9</v>
@@ -900,15 +909,15 @@
         <v>17</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
-      <c r="B3" s="31"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
@@ -922,12 +931,12 @@
         <v>25</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
-      <c r="B4" s="31"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
@@ -944,9 +953,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
-      <c r="B5" s="31"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
@@ -964,8 +973,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="31"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="5" t="s">
         <v>21</v>
       </c>
@@ -983,15 +992,15 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
-      <c r="B7" s="32" t="s">
+      <c r="A7" s="35"/>
+      <c r="B7" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>23</v>
@@ -1004,32 +1013,32 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>17</v>
@@ -1038,17 +1047,17 @@
         <v>24</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="32"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>18</v>
@@ -1060,35 +1069,35 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="32"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="33" t="s">
+      <c r="A12" s="35"/>
+      <c r="B12" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>23</v>
@@ -1101,51 +1110,51 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="33"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="19" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>18</v>
@@ -1157,35 +1166,35 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="33"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="29" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="31" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>23</v>
@@ -1198,51 +1207,51 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="21" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="21" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="22" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="29"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
-      <c r="B20" s="29"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="21" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>18</v>
@@ -1254,35 +1263,35 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="29"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="27" t="s">
+      <c r="A22" s="35"/>
+      <c r="B22" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>23</v>
@@ -1295,32 +1304,32 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>17</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="13" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>17</v>
@@ -1329,17 +1338,17 @@
         <v>24</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
-      <c r="B25" s="27"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="23" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>18</v>
@@ -1352,34 +1361,34 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="28" t="s">
-        <v>38</v>
+      <c r="A27" s="35"/>
+      <c r="B27" s="30" t="s">
+        <v>36</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>23</v>
@@ -1392,51 +1401,51 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E28" s="25" t="s">
         <v>17</v>
       </c>
       <c r="F28" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="G28" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>81</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="25" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E30" s="25" t="s">
         <v>18</v>
@@ -1449,26 +1458,89 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>19</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G31" s="16" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="28"/>
+      <c r="C33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="28"/>
+      <c r="C34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="27"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B32:B34"/>
     <mergeCell ref="B22:B26"/>
     <mergeCell ref="B27:B31"/>
     <mergeCell ref="B17:B21"/>

</xml_diff>